<commit_message>
-add readme -update analysis file
</commit_message>
<xml_diff>
--- a/analiz_sonuclari.xlsx
+++ b/analiz_sonuclari.xlsx
@@ -454,27 +454,27 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Bitki</t>
+          <t>Laptop</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Futbol Topu</t>
+          <t>Araç Aksesuarı</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Araç Aksesuarı</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -488,13 +488,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Kalem</t>
+          <t>Futbol Topu</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -504,7 +504,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Lego</t>
+          <t>T-shirt</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -514,41 +514,41 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Parfüm</t>
+          <t>Bitki</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Parfüm</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>T-shirt</t>
+          <t>Kalem</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Laptop</t>
+          <t>Lego</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -599,13 +599,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1211.107</v>
+        <v>942.8969999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>513.99</v>
+        <v>139.9</v>
       </c>
       <c r="D2" t="n">
-        <v>1966.3</v>
+        <v>1980.24</v>
       </c>
     </row>
     <row r="3">
@@ -615,13 +615,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3379.983999999999</v>
+        <v>2759.248</v>
       </c>
       <c r="C3" t="n">
-        <v>632.62</v>
+        <v>664.35</v>
       </c>
       <c r="D3" t="n">
-        <v>4884.69</v>
+        <v>4481.1</v>
       </c>
     </row>
     <row r="4">
@@ -631,13 +631,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1794.181</v>
+        <v>1404.047</v>
       </c>
       <c r="C4" t="n">
-        <v>478.07</v>
+        <v>155.92</v>
       </c>
       <c r="D4" t="n">
-        <v>2723.97</v>
+        <v>2779.23</v>
       </c>
     </row>
     <row r="5">
@@ -647,13 +647,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>220.792</v>
+        <v>285.283</v>
       </c>
       <c r="C5" t="n">
-        <v>94.40000000000001</v>
+        <v>97.42</v>
       </c>
       <c r="D5" t="n">
-        <v>397.4</v>
+        <v>480.88</v>
       </c>
     </row>
     <row r="6">
@@ -663,13 +663,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>86.92699999999999</v>
+        <v>93.304</v>
       </c>
       <c r="C6" t="n">
-        <v>31.26</v>
+        <v>49.24</v>
       </c>
       <c r="D6" t="n">
-        <v>149.12</v>
+        <v>134.66</v>
       </c>
     </row>
     <row r="7">
@@ -679,13 +679,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>157.199</v>
+        <v>181.148</v>
       </c>
       <c r="C7" t="n">
-        <v>62.35</v>
+        <v>104.04</v>
       </c>
       <c r="D7" t="n">
-        <v>268.17</v>
+        <v>268.8</v>
       </c>
     </row>
     <row r="8">
@@ -695,13 +695,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>47.00444444444445</v>
+        <v>63.673</v>
       </c>
       <c r="C8" t="n">
-        <v>11.04</v>
+        <v>19.38</v>
       </c>
       <c r="D8" t="n">
-        <v>95.37</v>
+        <v>92.54000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -711,13 +711,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>645.749</v>
+        <v>505.946</v>
       </c>
       <c r="C9" t="n">
-        <v>114.66</v>
+        <v>74.02</v>
       </c>
       <c r="D9" t="n">
-        <v>998.67</v>
+        <v>860.65</v>
       </c>
     </row>
     <row r="10">
@@ -727,13 +727,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>286.376</v>
+        <v>278.348</v>
       </c>
       <c r="C10" t="n">
-        <v>51.58</v>
+        <v>53.5</v>
       </c>
       <c r="D10" t="n">
-        <v>493.72</v>
+        <v>469.82</v>
       </c>
     </row>
     <row r="11">
@@ -743,13 +743,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1220.967</v>
+        <v>745.841</v>
       </c>
       <c r="C11" t="n">
-        <v>555.33</v>
+        <v>106</v>
       </c>
       <c r="D11" t="n">
-        <v>1934.88</v>
+        <v>1530.13</v>
       </c>
     </row>
   </sheetData>
@@ -763,7 +763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,81 +786,61 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Araç Aksesuarı</t>
+          <t>Kalem</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Bitki</t>
+          <t>Mobilya</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Lego</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Futbol Topu</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Parfüm</t>
+          <t>Laptop</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>T-shirt</t>
+          <t>Parfüm</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Futbol Topu</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Mobilya</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -906,10 +886,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C2" t="n">
-        <v>27639.79</v>
+        <v>32209.56</v>
       </c>
     </row>
     <row r="3">
@@ -919,10 +899,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C3" t="n">
-        <v>40540.96</v>
+        <v>55189.83</v>
       </c>
     </row>
     <row r="4">
@@ -932,10 +912,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C4" t="n">
-        <v>122634.41</v>
+        <v>53083.25</v>
       </c>
     </row>
     <row r="5">
@@ -945,10 +925,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>50574.33888888889</v>
+        <v>77033.36</v>
       </c>
     </row>
     <row r="6">
@@ -961,7 +941,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="n">
-        <v>32169.27</v>
+        <v>25227.16</v>
       </c>
     </row>
   </sheetData>
@@ -998,33 +978,33 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>product_name</t>
+          <t>quantity</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>purchase_date</t>
+          <t>satisfaction_score</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>price</t>
+          <t>purchase_date</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1037,7 +1017,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>customer_id</t>
+          <t>product_name</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1050,7 +1030,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>customer_id</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1063,7 +1043,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>category</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1076,7 +1056,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>quantity</t>
+          <t>price</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1089,7 +1069,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>satisfaction_score</t>
+          <t>category</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1213,13 +1193,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1245,13 +1225,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1277,13 +1257,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -1293,13 +1273,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -1391,7 +1371,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1089.9963</v>
+        <v>1037.1867</v>
       </c>
     </row>
     <row r="3">
@@ -1404,7 +1384,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3041.9856</v>
+        <v>3035.1728</v>
       </c>
     </row>
     <row r="4">
@@ -1417,7 +1397,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1973.5991</v>
+        <v>1263.6423</v>
       </c>
     </row>
     <row r="5">
@@ -1430,7 +1410,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>242.8712</v>
+        <v>313.8113</v>
       </c>
     </row>
     <row r="6">
@@ -1443,7 +1423,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>95.61969999999999</v>
+        <v>102.6344</v>
       </c>
     </row>
     <row r="7">
@@ -1456,7 +1436,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>172.9189</v>
+        <v>163.0332</v>
       </c>
     </row>
     <row r="8">
@@ -1469,7 +1449,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>51.7048888888889</v>
+        <v>57.3057</v>
       </c>
     </row>
     <row r="9">
@@ -1482,7 +1462,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>710.3239000000001</v>
+        <v>455.3514</v>
       </c>
     </row>
     <row r="10">
@@ -1495,7 +1475,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>315.0136000000001</v>
+        <v>306.1828</v>
       </c>
     </row>
     <row r="11">
@@ -1508,7 +1488,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1343.0637</v>
+        <v>671.2569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Update dynamic price function
</commit_message>
<xml_diff>
--- a/analiz_sonuclari.xlsx
+++ b/analiz_sonuclari.xlsx
@@ -454,101 +454,101 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Laptop</t>
+          <t>Mutfak Eşyası</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Araç Aksesuarı</t>
+          <t>Sulama Sistemi</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Araç Aksesuarı</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Mobilya</t>
+          <t>Bahçe Aletleri</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Futbol Topu</t>
+          <t>Dekorasyon</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>T-shirt</t>
+          <t>Klavye</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Bitki</t>
+          <t>Bisiklet</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Parfüm</t>
+          <t>Çanta</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Kalem</t>
+          <t>Tenis Raketi</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Lego</t>
+          <t>Akademik</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -599,13 +599,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>942.8969999999999</v>
+        <v>893.5477192982456</v>
       </c>
       <c r="C2" t="n">
-        <v>139.9</v>
+        <v>103.34</v>
       </c>
       <c r="D2" t="n">
-        <v>1980.24</v>
+        <v>1995.58</v>
       </c>
     </row>
     <row r="3">
@@ -615,13 +615,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2759.248</v>
+        <v>2774.251754385965</v>
       </c>
       <c r="C3" t="n">
-        <v>664.35</v>
+        <v>526.98</v>
       </c>
       <c r="D3" t="n">
-        <v>4481.1</v>
+        <v>4993.84</v>
       </c>
     </row>
     <row r="4">
@@ -631,13 +631,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1404.047</v>
+        <v>1435.741178369653</v>
       </c>
       <c r="C4" t="n">
-        <v>155.92</v>
+        <v>132.78</v>
       </c>
       <c r="D4" t="n">
-        <v>2779.23</v>
+        <v>2999.64</v>
       </c>
     </row>
     <row r="5">
@@ -647,13 +647,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>285.283</v>
+        <v>237.8455357142857</v>
       </c>
       <c r="C5" t="n">
-        <v>97.42</v>
+        <v>56.6</v>
       </c>
       <c r="D5" t="n">
-        <v>480.88</v>
+        <v>473.58</v>
       </c>
     </row>
     <row r="6">
@@ -663,13 +663,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>93.304</v>
+        <v>87.4574358974359</v>
       </c>
       <c r="C6" t="n">
-        <v>49.24</v>
+        <v>22.7</v>
       </c>
       <c r="D6" t="n">
-        <v>134.66</v>
+        <v>154.85</v>
       </c>
     </row>
     <row r="7">
@@ -679,13 +679,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>181.148</v>
+        <v>178.5532075471698</v>
       </c>
       <c r="C7" t="n">
-        <v>104.04</v>
+        <v>32.93</v>
       </c>
       <c r="D7" t="n">
-        <v>268.8</v>
+        <v>299.45</v>
       </c>
     </row>
     <row r="8">
@@ -695,13 +695,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>63.673</v>
+        <v>46.61862068965517</v>
       </c>
       <c r="C8" t="n">
-        <v>19.38</v>
+        <v>6.21</v>
       </c>
       <c r="D8" t="n">
-        <v>92.54000000000001</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="9">
@@ -711,13 +711,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>505.946</v>
+        <v>562.9056923076923</v>
       </c>
       <c r="C9" t="n">
-        <v>74.02</v>
+        <v>77.73</v>
       </c>
       <c r="D9" t="n">
-        <v>860.65</v>
+        <v>998.67</v>
       </c>
     </row>
     <row r="10">
@@ -727,13 +727,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>278.348</v>
+        <v>260.8737391304348</v>
       </c>
       <c r="C10" t="n">
-        <v>53.5</v>
+        <v>63.71</v>
       </c>
       <c r="D10" t="n">
-        <v>469.82</v>
+        <v>514.8</v>
       </c>
     </row>
     <row r="11">
@@ -743,13 +743,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>745.841</v>
+        <v>1005.694345238095</v>
       </c>
       <c r="C11" t="n">
-        <v>106</v>
+        <v>171.02</v>
       </c>
       <c r="D11" t="n">
-        <v>1530.13</v>
+        <v>1974.15</v>
       </c>
     </row>
   </sheetData>
@@ -763,7 +763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,61 +786,391 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Kalem</t>
+          <t>Biyografi</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Mobilya</t>
+          <t>Koşu Ayakkabısı</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Mouse</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Futbol Topu</t>
+          <t>Tenis Raketi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Laptop</t>
+          <t>Ev Tekstili</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
+          <t>Çanta</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Ajanda</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Defter</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Tablet</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Yoga Matı</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Puzzle</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Bisiklet</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Sulama Sistemi</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Gömlek</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Kişisel Gelişim</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Perde</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Pantolon</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Futbol Topu</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Araç Aksesuarı</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Monitör</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Klavye</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Elbise</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Akıllı Telefon</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Şampuan</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Bahçe Aletleri</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Oyun Konsolu</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Oto Parfümü</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Kulaklık</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Güneş Kremi</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
           <t>Parfüm</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>4</v>
+      <c r="B31" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>Şapka</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>Tarih</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>Makyaj Seti</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Uzaktan Kumandalı Araba</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>Bitki</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>Boya Seti</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Dergi</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Yağ</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -886,10 +1216,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C2" t="n">
-        <v>32209.56</v>
+        <v>279417.5514285714</v>
       </c>
     </row>
     <row r="3">
@@ -899,10 +1229,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="C3" t="n">
-        <v>55189.83</v>
+        <v>321983.48</v>
       </c>
     </row>
     <row r="4">
@@ -912,10 +1242,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="C4" t="n">
-        <v>53083.25</v>
+        <v>225420.4833333333</v>
       </c>
     </row>
     <row r="5">
@@ -925,10 +1255,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="C5" t="n">
-        <v>77033.36</v>
+        <v>336205.8333333334</v>
       </c>
     </row>
     <row r="6">
@@ -938,10 +1268,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="C6" t="n">
-        <v>25227.16</v>
+        <v>247446.3386666666</v>
       </c>
     </row>
   </sheetData>
@@ -978,40 +1308,40 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>quantity</t>
+          <t>satisfaction_score</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>17.3109243697479</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>satisfaction_score</t>
+          <t>purchase_date</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1.344537815126051</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>purchase_date</t>
+          <t>price</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>1.008403361344538</v>
       </c>
     </row>
     <row r="5">
@@ -1056,7 +1386,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>price</t>
+          <t>category</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1069,7 +1399,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>category</t>
+          <t>quantity</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1225,13 +1555,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -1241,13 +1571,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -1257,13 +1587,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1273,13 +1603,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10">
@@ -1341,7 +1671,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1367,11 +1697,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bitki</t>
+          <t>Akıllı Telefon</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1037.1867</v>
+        <v>3051.68</v>
       </c>
     </row>
     <row r="3">
@@ -1380,11 +1710,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Laptop</t>
+          <t>Kamera</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3035.1728</v>
+        <v>2775.02</v>
       </c>
     </row>
     <row r="4">
@@ -1393,11 +1723,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mobilya</t>
+          <t>Klavye</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1263.6423</v>
+        <v>3051.68</v>
       </c>
     </row>
     <row r="5">
@@ -1406,11 +1736,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>T-shirt</t>
+          <t>Kulaklık</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>313.8113</v>
+        <v>2496.83</v>
       </c>
     </row>
     <row r="6">
@@ -1419,11 +1749,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>Laptop</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>102.6344</v>
+        <v>2496.83</v>
       </c>
     </row>
     <row r="7">
@@ -1432,11 +1762,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Parfüm</t>
+          <t>Tablet</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>163.0332</v>
+        <v>3051.68</v>
       </c>
     </row>
     <row r="8">
@@ -1445,11 +1775,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Kalem</t>
+          <t>Ayakkabı</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>57.3057</v>
+        <v>261.63</v>
       </c>
     </row>
     <row r="9">
@@ -1458,11 +1788,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Araç Aksesuarı</t>
+          <t>Ceket</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>455.3514</v>
+        <v>214.06</v>
       </c>
     </row>
     <row r="10">
@@ -1471,11 +1801,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lego</t>
+          <t>Gömlek</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>306.1828</v>
+        <v>214.06</v>
       </c>
     </row>
     <row r="11">
@@ -1484,11 +1814,440 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Futbol Topu</t>
+          <t>T-shirt</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>671.2569</v>
+        <v>214.06</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Çanta</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>214.06</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Şapka</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>261.63</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bilim Kurgu</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>96.2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Biyografi</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>96.2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Kişisel Gelişim</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>78.70999999999999</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Roman</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>78.70999999999999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Tarih</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>78.70999999999999</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Çocuk Kitabı</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>96.2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Bisiklet</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>905.12</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Spor Çantası</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1106.26</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Tenis Raketi</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>905.12</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Yüzme Gözlüğü</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1106.26</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Aydınlatma</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1579.32</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Dekorasyon</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1292.17</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Halı</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1292.17</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Mutfak Eşyası</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1579.32</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Perde</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>1292.17</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Krem</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>160.7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Parfüm</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>196.41</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Ruj</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>160.7</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Şampuan</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>196.41</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Bebek</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>234.79</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Eğitici Oyuncak</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>286.96</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>234.79</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Peluş Oyuncak</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>234.79</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Bahçe Aletleri</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>804.1900000000001</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Gübre</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>982.9</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Saksı</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>982.9</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Tohum</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>804.1900000000001</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Ajanda</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>51.28</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Boya Seti</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>41.96</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Defter</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>41.96</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Dosya</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>51.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>